<commit_message>
Update documentaion with 12.07.2017 updates
</commit_message>
<xml_diff>
--- a/src/_static/xlsx/tab_aggiornamenti_alla_documentazione_tecnica.xlsx
+++ b/src/_static/xlsx/tab_aggiornamenti_alla_documentazione_tecnica.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20220" windowHeight="8040"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19440" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="aggiornamenti_20_01_2017" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="127">
   <si>
     <t>documenti aggiornati</t>
   </si>
@@ -316,10 +316,85 @@
     <t>errori_anpr_16_05_2017.xlsx</t>
   </si>
   <si>
-    <t>tabella_1_stato_civile.xlsx</t>
-  </si>
-  <si>
-    <t>Modificate le codifiche 7 e 8 (sono state invertite)</t>
+    <t>wsdlN000</t>
+  </si>
+  <si>
+    <t>wsdl6001</t>
+  </si>
+  <si>
+    <t>Certificazioni</t>
+  </si>
+  <si>
+    <t>wsdl1000</t>
+  </si>
+  <si>
+    <t>1002-IscrizioneAltriMotivi</t>
+  </si>
+  <si>
+    <t>A001-IscrizioneAIRENascita</t>
+  </si>
+  <si>
+    <t>wsdl5000</t>
+  </si>
+  <si>
+    <t>5001-MutazioneFamiglia-Convivenza</t>
+  </si>
+  <si>
+    <t>5012-AnnullamentoMutazione</t>
+  </si>
+  <si>
+    <t>Tracciati XSD e WSDL - rar</t>
+  </si>
+  <si>
+    <t>Specifiche di interfaccia dei servizi di ANPR per i comuni – documentazione tecnica - rar</t>
+  </si>
+  <si>
+    <t>Inserite le notifiche N014 ed N015</t>
+  </si>
+  <si>
+    <t>Aggiunti commenti per alcuni campi</t>
+  </si>
+  <si>
+    <t>Specificati i valori attualmente utilizzati della lista controlli</t>
+  </si>
+  <si>
+    <t>Eliminati CC071, CN303 e CN308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggiornamento tabelle decodifica </t>
+  </si>
+  <si>
+    <t>Aggiornamento tabelle 24 e 41 consolati e territori</t>
+  </si>
+  <si>
+    <t>Riapertura consolato Santo Domingo 2690100</t>
+  </si>
+  <si>
+    <t>5013-RevocaDato</t>
+  </si>
+  <si>
+    <t>Aggiornati i file vocabolario5000mutazione.xsd, 5000mutazione.xsd, tipoDato.xsd</t>
+  </si>
+  <si>
+    <t>Aggiounti i file 5013-RevocaDato.xlsx, revocaDato.xlsx, schedaSoggetto.xlsx</t>
+  </si>
+  <si>
+    <t>Risoluzione disallineamenti con l'Agenzia delle Entrate 12_07_2017.pdf</t>
+  </si>
+  <si>
+    <t>Appendice al documento di specifiche</t>
+  </si>
+  <si>
+    <t>errori_anpr_12_07_2017.xlsx</t>
+  </si>
+  <si>
+    <t>Residenza estera</t>
+  </si>
+  <si>
+    <t>alfanumerico120char</t>
+  </si>
+  <si>
+    <t>Non è più ammesso il carattere "/" per Località e Indirizzo estero</t>
   </si>
 </sst>
 </file>
@@ -825,7 +900,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -848,6 +923,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1191,16 +1269,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1875,7 +1953,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>42866</v>
       </c>
@@ -1975,16 +2053,282 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
-        <v>42866</v>
-      </c>
-      <c r="B57" s="8" t="s">
+        <v>42907</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
+        <v>42907</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
+        <v>42912</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>42928</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <v>42928</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
+        <v>42928</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
+        <v>42928</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <v>42928</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="7">
+        <v>42928</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>101</v>
+      <c r="C76" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1994,21 +2338,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0EB43895666D743BBE5EE80DE8AFF2D" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3898ec998cc85d3bcc261598fbbf3dc9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -2122,17 +2451,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{872D4FEA-0E1A-4A2F-890F-971ABD26DD30}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30A4E566-AAC9-451E-AA26-97377196906E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2146,17 +2491,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30A4E566-AAC9-451E-AA26-97377196906E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{872D4FEA-0E1A-4A2F-890F-971ABD26DD30}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Anpr technical documentation - code errors
</commit_message>
<xml_diff>
--- a/src/_static/xlsx/tab_aggiornamenti_alla_documentazione_tecnica.xlsx
+++ b/src/_static/xlsx/tab_aggiornamenti_alla_documentazione_tecnica.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="19440" windowHeight="8040"/>
   </bookViews>
   <sheets>
-    <sheet name="aggiornamenti_20_01_2017" sheetId="1" r:id="rId1"/>
+    <sheet name="aggiornamenti_29_08_2017" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="137">
   <si>
     <t>documenti aggiornati</t>
   </si>
@@ -376,9 +376,6 @@
     <t>Aggiornati i file vocabolario5000mutazione.xsd, 5000mutazione.xsd, tipoDato.xsd</t>
   </si>
   <si>
-    <t>Aggiounti i file 5013-RevocaDato.xlsx, revocaDato.xlsx, schedaSoggetto.xlsx</t>
-  </si>
-  <si>
     <t>Risoluzione disallineamenti con l'Agenzia delle Entrate 12_07_2017.pdf</t>
   </si>
   <si>
@@ -395,6 +392,43 @@
   </si>
   <si>
     <t>Non è più ammesso il carattere "/" per Località e Indirizzo estero</t>
+  </si>
+  <si>
+    <t>errori_anpr_31_08_2017.xlsx</t>
+  </si>
+  <si>
+    <t>Aggiunti i file 5013-RevocaDato.xlsx, revocaDato.xlsx, schedaSoggetto.xlsx</t>
+  </si>
+  <si>
+    <t>In 6001-RichiestaCertificati.xlsx  aggiunto forzaCertificazione già presente nell'XSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contratto Risoluzione.xlsx
+scioglimentoUnione.xlsx
+Specificato utilizzo del cod. motivo scioglimento 98 = Decesso del convivente/unito civilmente </t>
+  </si>
+  <si>
+    <t>In 5005-MutazioneResidenza.xlsx  aggiunto valore per forzare il cambio di residenza allo stesso indirizzo</t>
+  </si>
+  <si>
+    <t>errori_anpr_20170922.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserimento/Aggiornamento codici di errore di ANPR 
+</t>
+  </si>
+  <si>
+    <t>Oggetti</t>
+  </si>
+  <si>
+    <t>localitaEstera.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specificato che nel campo descrizioneConsolato deve essere riportata la città Sede del consolato come da tabella 24
+</t>
+  </si>
+  <si>
+    <t>errori_anpr_20170928.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1269,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,13 +2300,13 @@
         <v>42928</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="D72" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2286,7 +2320,7 @@
         <v>110</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2311,10 +2345,10 @@
         <v>68</v>
       </c>
       <c r="C75" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2325,10 +2359,122 @@
         <v>57</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
+        <v>42978</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <v>42978</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
+        <v>42978</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="7">
+        <v>42983</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="7">
+        <v>42983</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
+        <v>43000</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
+        <v>43000</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="7">
+        <v>43006</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2493,14 +2639,14 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{872D4FEA-0E1A-4A2F-890F-971ABD26DD30}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add new documentation and fix error for tabella Relazione Parentela
</commit_message>
<xml_diff>
--- a/src/_static/xlsx/tab_aggiornamenti_alla_documentazione_tecnica.xlsx
+++ b/src/_static/xlsx/tab_aggiornamenti_alla_documentazione_tecnica.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="161">
   <si>
     <t>documenti aggiornati</t>
   </si>
@@ -429,6 +429,87 @@
   </si>
   <si>
     <t>errori_anpr_20170928.xlsx</t>
+  </si>
+  <si>
+    <t>tabella 3 archivio comuni 20171005.xlsx</t>
+  </si>
+  <si>
+    <t>Tabella 3 comuni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La denominazione per MONTEBELLO IONICO diventa MONTEBELLO JONICO 
+Il codice catastale del comune CASALI DEL MANCO è impostato a M385 (prima era N.D, i.e. Non Disponibile)
+Il codice catastale per OLGIATE CALCO (due record) diventa G027 (prima era G026) in accordo a quanto presente nella banca dati di AE
+</t>
+  </si>
+  <si>
+    <t>errori_anpr_05102017.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserimento codice di errore EN407, EN427
+</t>
+  </si>
+  <si>
+    <t>errori_anpr_11102017.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminato codice di errore EN375 dal servizio 2003
+</t>
+  </si>
+  <si>
+    <t>tipoDatiControllo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggiornato il file vocabolario5000mutazione.xsd per documentare l'utilizzo dei dati di controllo </t>
+  </si>
+  <si>
+    <t>errori_anpr_16102017.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il codice di errore EC039 è attivo anche per il subentro
+</t>
+  </si>
+  <si>
+    <t>In Allegato XML S001- Subentro.xls specificate regole/condizioni per convivenza e responsabile convivenza</t>
+  </si>
+  <si>
+    <t>errori_anpr_18102017.xlsx</t>
+  </si>
+  <si>
+    <t>Inserimento codice di errore EN436</t>
+  </si>
+  <si>
+    <t>errori_anpr_19102017.xlsx</t>
+  </si>
+  <si>
+    <t>Inserimento codice di errore EN411</t>
+  </si>
+  <si>
+    <t>Invio file di Subentro</t>
+  </si>
+  <si>
+    <t>Aggiornate istruzioni per la predisposizione del file AIRE con AnagAire 6.0.3</t>
+  </si>
+  <si>
+    <t>Sito WEB di ANPR e specifiche di integrazione.pdf</t>
+  </si>
+  <si>
+    <t>Allegato 2 - Elenco funzioni WEB19102017.xlsx</t>
+  </si>
+  <si>
+    <t>Allegato 7 - Utilizzo WS ANPR totale 19102017.xlsx</t>
+  </si>
+  <si>
+    <t>Inserita la descrizione delle seguenti funzioni:
+Registrazione/Eliminazione dati
+Registrazione/Rettifiche
+Consultazione/Consultazione AE</t>
+  </si>
+  <si>
+    <t>Inserita operazione anagrafica 4002</t>
+  </si>
+  <si>
+    <t>Documentazione sito WEB</t>
   </si>
 </sst>
 </file>
@@ -1303,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95:B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,6 +2558,174 @@
         <v>132</v>
       </c>
     </row>
+    <row r="85" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="7">
+        <v>42865</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="7">
+        <v>42865</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="7">
+        <v>43019</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
+        <v>43019</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
+        <v>43024</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
+        <v>43025</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
+        <v>43026</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="7">
+        <v>43027</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D92" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="7">
+        <v>43027</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
+        <v>43027</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A95" s="7">
+        <v>43027</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
+        <v>43027</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2484,6 +2733,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0EB43895666D743BBE5EE80DE8AFF2D" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3898ec998cc85d3bcc261598fbbf3dc9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -2597,22 +2861,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{872D4FEA-0E1A-4A2F-890F-971ABD26DD30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{166CB6B4-1638-4D05-A349-B472930EF1EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30A4E566-AAC9-451E-AA26-97377196906E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2626,27 +2898,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{166CB6B4-1638-4D05-A349-B472930EF1EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{872D4FEA-0E1A-4A2F-890F-971ABD26DD30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add the updated documentation for ANPR
</commit_message>
<xml_diff>
--- a/src/_static/xlsx/tab_aggiornamenti_alla_documentazione_tecnica.xlsx
+++ b/src/_static/xlsx/tab_aggiornamenti_alla_documentazione_tecnica.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="19440" windowHeight="8040"/>
   </bookViews>
   <sheets>
-    <sheet name="aggiornamenti_29_08_2017" sheetId="1" r:id="rId1"/>
+    <sheet name="aggiornamenti_14_11_2017" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="171">
   <si>
     <t>documenti aggiornati</t>
   </si>
@@ -510,6 +510,36 @@
   </si>
   <si>
     <t>Documentazione sito WEB</t>
+  </si>
+  <si>
+    <t>errori_anpr_20171024.xlsx</t>
+  </si>
+  <si>
+    <t>tabella_46_tipo_mutazione_famiglia_convivenza.xlsx</t>
+  </si>
+  <si>
+    <t>tabella_47_tipo_mutazione_residenza.xlsx</t>
+  </si>
+  <si>
+    <t>Inserimento codici di errore EN416, EN426</t>
+  </si>
+  <si>
+    <t>errori_anpr_20171026.xlsx</t>
+  </si>
+  <si>
+    <t>Inserimento codice di errore EN447</t>
+  </si>
+  <si>
+    <t>errori_anpr_20171103.xlsx</t>
+  </si>
+  <si>
+    <t>errori_anpr_20171109.xlsx</t>
+  </si>
+  <si>
+    <t>Inserimento/Aggiornamento codici di errore di ANPR</t>
+  </si>
+  <si>
+    <t>errori_anpr_20171116.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1384,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95:B96"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,6 +2756,128 @@
         <v>159</v>
       </c>
     </row>
+    <row r="97" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <v>43032</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <v>43032</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <v>43032</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
+        <v>43032</v>
+      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
+        <v>43034</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D101" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
+        <v>43042</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="7">
+        <v>43042</v>
+      </c>
+      <c r="B103" s="1"/>
+      <c r="C103" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="7">
+        <v>43048</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="7">
+        <v>43055</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2733,21 +2885,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0EB43895666D743BBE5EE80DE8AFF2D" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3898ec998cc85d3bcc261598fbbf3dc9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -2861,17 +2998,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{872D4FEA-0E1A-4A2F-890F-971ABD26DD30}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30A4E566-AAC9-451E-AA26-97377196906E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2885,17 +3038,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30A4E566-AAC9-451E-AA26-97377196906E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{872D4FEA-0E1A-4A2F-890F-971ABD26DD30}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>